<commit_message>
tables and plot for problem 3
</commit_message>
<xml_diff>
--- a/data files/Trash-Wheel-Collection-Totals-8-6-19.xlsx
+++ b/data files/Trash-Wheel-Collection-Totals-8-6-19.xlsx
@@ -8,24 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shainamackin/Desktop/Fall 2021/Data Science I/HW 2/HW2/data files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5F471-E443-6A4F-AF93-BBB420D33113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BBBFA1-4B54-444A-B0C2-5C408729A30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31740" yWindow="2320" windowWidth="28800" windowHeight="16720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36760" yWindow="3960" windowWidth="36760" windowHeight="16720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mr. Trash Wheel" sheetId="3" r:id="rId1"/>
-    <sheet name="Professor Trash Wheel" sheetId="9" r:id="rId2"/>
-    <sheet name="Captain Trash Wheel" sheetId="11" r:id="rId3"/>
-    <sheet name="2019 Precipitation" sheetId="12" r:id="rId4"/>
-    <sheet name="2018 Precipitation" sheetId="10" r:id="rId5"/>
-    <sheet name="2017 Precipitation" sheetId="8" r:id="rId6"/>
-    <sheet name="2016 Precipitation" sheetId="6" r:id="rId7"/>
-    <sheet name="2015 Precipitation" sheetId="4" r:id="rId8"/>
-    <sheet name="2014 Precipitation" sheetId="2" r:id="rId9"/>
-    <sheet name="Homes powered note" sheetId="5" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
+    <sheet name="Professor Trash Wheel" sheetId="9" r:id="rId3"/>
+    <sheet name="Captain Trash Wheel" sheetId="11" r:id="rId4"/>
+    <sheet name="2019 Precipitation" sheetId="12" r:id="rId5"/>
+    <sheet name="2018 Precipitation" sheetId="10" r:id="rId6"/>
+    <sheet name="2017 Precipitation" sheetId="8" r:id="rId7"/>
+    <sheet name="2016 Precipitation" sheetId="6" r:id="rId8"/>
+    <sheet name="2015 Precipitation" sheetId="4" r:id="rId9"/>
+    <sheet name="2014 Precipitation" sheetId="2" r:id="rId10"/>
+    <sheet name="Homes powered note" sheetId="5" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mr. Trash Wheel'!$A$1:$O$294</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="50">
   <si>
     <t>Dumpster</t>
   </si>
@@ -197,6 +199,9 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>balls</t>
+  </si>
 </sst>
 </file>
 
@@ -337,7 +342,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -382,6 +387,19 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -768,7 +786,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1154,6 +1172,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="381">
@@ -2155,10 +2179,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DL454"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A401" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A405" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="M372" sqref="M372:M407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2171,7 +2195,8 @@
     <col min="6" max="6" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" style="26" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.5" style="26" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="27"/>
@@ -20260,7 +20285,7 @@
       </c>
       <c r="O384" s="72"/>
     </row>
-    <row r="385" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A385" s="41">
         <v>325</v>
       </c>
@@ -20306,7 +20331,7 @@
       </c>
       <c r="O385" s="91"/>
     </row>
-    <row r="386" spans="1:15" s="66" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:17" s="66" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A386" s="41">
         <v>326</v>
       </c>
@@ -20352,7 +20377,7 @@
       </c>
       <c r="O386" s="65"/>
     </row>
-    <row r="387" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A387" s="41">
         <v>327</v>
       </c>
@@ -20398,7 +20423,7 @@
       </c>
       <c r="O387" s="91"/>
     </row>
-    <row r="388" spans="1:15" s="67" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:17" s="67" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A388" s="41">
         <v>328</v>
       </c>
@@ -20444,7 +20469,7 @@
       </c>
       <c r="O388" s="68"/>
     </row>
-    <row r="389" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A389" s="41">
         <v>329</v>
       </c>
@@ -20490,7 +20515,7 @@
       </c>
       <c r="O389" s="91"/>
     </row>
-    <row r="390" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A390" s="41">
         <v>330</v>
       </c>
@@ -20535,8 +20560,9 @@
         <v>58.833333333333336</v>
       </c>
       <c r="O390" s="91"/>
-    </row>
-    <row r="391" spans="1:15" s="36" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q390" s="84"/>
+    </row>
+    <row r="391" spans="1:17" s="36" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A391" s="49"/>
       <c r="B391" s="49" t="s">
         <v>43</v>
@@ -20584,8 +20610,9 @@
         <v>363.66666666666663</v>
       </c>
       <c r="O391" s="92"/>
-    </row>
-    <row r="392" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q391" s="134"/>
+    </row>
+    <row r="392" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A392" s="41">
         <v>331</v>
       </c>
@@ -20630,8 +20657,9 @@
         <v>50.666666666666664</v>
       </c>
       <c r="O392" s="91"/>
-    </row>
-    <row r="393" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q392" s="135"/>
+    </row>
+    <row r="393" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A393" s="41">
         <v>332</v>
       </c>
@@ -20676,8 +20704,9 @@
         <v>51.166666666666664</v>
       </c>
       <c r="O393" s="91"/>
-    </row>
-    <row r="394" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q393" s="134"/>
+    </row>
+    <row r="394" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A394" s="41">
         <v>333</v>
       </c>
@@ -20722,8 +20751,9 @@
         <v>53.833333333333336</v>
       </c>
       <c r="O394" s="91"/>
-    </row>
-    <row r="395" spans="1:15" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q394" s="134"/>
+    </row>
+    <row r="395" spans="1:17" s="34" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A395" s="41">
         <v>334</v>
       </c>
@@ -20768,8 +20798,9 @@
         <v>62.166666666666664</v>
       </c>
       <c r="O395" s="91"/>
-    </row>
-    <row r="396" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q395" s="135"/>
+    </row>
+    <row r="396" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A396" s="41">
         <v>335</v>
       </c>
@@ -20814,8 +20845,9 @@
         <v>56.333333333333336</v>
       </c>
       <c r="O396" s="77"/>
-    </row>
-    <row r="397" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q396" s="134"/>
+    </row>
+    <row r="397" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A397" s="41">
         <v>336</v>
       </c>
@@ -20860,8 +20892,9 @@
         <v>48.666666666666664</v>
       </c>
       <c r="O397" s="77"/>
-    </row>
-    <row r="398" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q397" s="134"/>
+    </row>
+    <row r="398" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A398" s="41">
         <v>337</v>
       </c>
@@ -20906,8 +20939,9 @@
         <v>47.166666666666664</v>
       </c>
       <c r="O398" s="77"/>
-    </row>
-    <row r="399" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q398" s="134"/>
+    </row>
+    <row r="399" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A399" s="41">
         <v>338</v>
       </c>
@@ -20952,8 +20986,9 @@
         <v>46</v>
       </c>
       <c r="O399" s="77"/>
-    </row>
-    <row r="400" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q399" s="134"/>
+    </row>
+    <row r="400" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A400" s="41">
         <v>339</v>
       </c>
@@ -20998,8 +21033,9 @@
         <v>41.833333333333336</v>
       </c>
       <c r="O400" s="77"/>
-    </row>
-    <row r="401" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q400" s="134"/>
+    </row>
+    <row r="401" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A401" s="41">
         <v>340</v>
       </c>
@@ -21044,8 +21080,9 @@
         <v>45.333333333333336</v>
       </c>
       <c r="O401" s="77"/>
-    </row>
-    <row r="402" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q401" s="134"/>
+    </row>
+    <row r="402" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A402" s="41">
         <v>341</v>
       </c>
@@ -21090,8 +21127,9 @@
         <v>53.166666666666664</v>
       </c>
       <c r="O402" s="77"/>
-    </row>
-    <row r="403" spans="1:15" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q402" s="135"/>
+    </row>
+    <row r="403" spans="1:17" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A403" s="49"/>
       <c r="B403" s="49" t="s">
         <v>45</v>
@@ -21139,8 +21177,9 @@
         <v>556.33333333333326</v>
       </c>
       <c r="O403" s="72"/>
-    </row>
-    <row r="404" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q403" s="134"/>
+    </row>
+    <row r="404" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A404" s="41">
         <v>342</v>
       </c>
@@ -21185,8 +21224,9 @@
         <v>53.833333333333336</v>
       </c>
       <c r="O404" s="77"/>
-    </row>
-    <row r="405" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q404" s="134"/>
+    </row>
+    <row r="405" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A405" s="41">
         <v>343</v>
       </c>
@@ -21231,8 +21271,9 @@
         <v>51.333333333333336</v>
       </c>
       <c r="O405" s="77"/>
-    </row>
-    <row r="406" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="Q405" s="134"/>
+    </row>
+    <row r="406" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A406" s="41">
         <v>344</v>
       </c>
@@ -21277,8 +21318,9 @@
         <v>50.333333333333336</v>
       </c>
       <c r="O406" s="77"/>
-    </row>
-    <row r="407" spans="1:15" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q406" s="134"/>
+    </row>
+    <row r="407" spans="1:17" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A407" s="49"/>
       <c r="B407" s="49" t="s">
         <v>33</v>
@@ -21326,8 +21368,9 @@
         <v>155.5</v>
       </c>
       <c r="O407" s="72"/>
-    </row>
-    <row r="408" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q407" s="134"/>
+    </row>
+    <row r="408" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A408" s="57"/>
       <c r="B408" s="57" t="s">
         <v>46</v>
@@ -21375,31 +21418,66 @@
         <v>15075.833333333332</v>
       </c>
       <c r="O408" s="99"/>
-    </row>
-    <row r="409" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="410" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="411" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="412" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="413" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="414" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="415" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="416" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="417" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="418" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="419" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="420" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="421" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="422" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="423" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="424" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="425" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="426" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="427" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="428" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="429" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="430" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="431" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="432" outlineLevel="1" x14ac:dyDescent="0.2"/>
+      <c r="Q408" s="134"/>
+    </row>
+    <row r="409" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q409" s="135"/>
+    </row>
+    <row r="410" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q410" s="134"/>
+    </row>
+    <row r="411" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q411" s="134"/>
+    </row>
+    <row r="412" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q412" s="134"/>
+    </row>
+    <row r="413" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q413" s="134"/>
+    </row>
+    <row r="414" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q414" s="134"/>
+    </row>
+    <row r="415" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q415" s="134"/>
+    </row>
+    <row r="416" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q416" s="134"/>
+    </row>
+    <row r="417" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q417" s="134"/>
+    </row>
+    <row r="418" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q418" s="134"/>
+    </row>
+    <row r="419" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q419" s="134"/>
+    </row>
+    <row r="420" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q420" s="134"/>
+    </row>
+    <row r="421" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q421" s="135"/>
+    </row>
+    <row r="422" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q422" s="134"/>
+    </row>
+    <row r="423" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q423" s="134"/>
+    </row>
+    <row r="424" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q424" s="134"/>
+    </row>
+    <row r="425" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="Q425" s="135"/>
+    </row>
+    <row r="426" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="427" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="428" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="429" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="430" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="431" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="432" spans="17:17" outlineLevel="1" x14ac:dyDescent="0.2"/>
     <row r="433" spans="3:14" outlineLevel="1" x14ac:dyDescent="0.2"/>
     <row r="434" spans="3:14" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="C434" s="27"/>
@@ -21469,6 +21547,142 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f>SUM(B3:B14)</f>
+        <v>51.59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -21489,6 +21703,271 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35538896-39D3-DC44-A9E7-C219723D2293}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="49">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="49">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="49">
+        <v>2</v>
+      </c>
+      <c r="C4" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="49">
+        <v>3</v>
+      </c>
+      <c r="C5" s="41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="49">
+        <v>4</v>
+      </c>
+      <c r="C6" s="41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="49">
+        <v>4</v>
+      </c>
+      <c r="C7" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="49">
+        <v>4</v>
+      </c>
+      <c r="C8" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="49">
+        <v>4</v>
+      </c>
+      <c r="C9" s="41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="49">
+        <v>6</v>
+      </c>
+      <c r="C10" s="41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="49">
+        <v>6</v>
+      </c>
+      <c r="C11" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="49">
+        <v>6</v>
+      </c>
+      <c r="C12" s="41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="49">
+        <v>8</v>
+      </c>
+      <c r="C13" s="41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="49">
+        <v>8</v>
+      </c>
+      <c r="C14" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="49">
+        <v>8</v>
+      </c>
+      <c r="C15" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="41">
+        <v>8</v>
+      </c>
+      <c r="C16" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="41">
+        <v>9</v>
+      </c>
+      <c r="C17" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="49">
+        <v>9</v>
+      </c>
+      <c r="C18" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="49">
+        <v>9</v>
+      </c>
+      <c r="C19" s="41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="49">
+        <v>10</v>
+      </c>
+      <c r="C20" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="49">
+        <v>11</v>
+      </c>
+      <c r="C21" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="49">
+        <v>11</v>
+      </c>
+      <c r="C22" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="49">
+        <v>13</v>
+      </c>
+      <c r="C23" s="41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="49">
+        <v>14</v>
+      </c>
+      <c r="C24" s="41">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="49">
+        <v>14</v>
+      </c>
+      <c r="C25" s="41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="49">
+        <v>14</v>
+      </c>
+      <c r="C26" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="49">
+        <v>14</v>
+      </c>
+      <c r="C27" s="41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="49">
+        <v>16</v>
+      </c>
+      <c r="C28" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="49">
+        <v>17</v>
+      </c>
+      <c r="C29" s="41">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="49">
+        <v>17</v>
+      </c>
+      <c r="C30" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="49">
+        <v>22</v>
+      </c>
+      <c r="C31" s="41">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A27" xr:uid="{35538896-39D3-DC44-A9E7-C219723D2293}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A31">
+      <sortCondition ref="A1:A31"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O213"/>
   <sheetViews>
@@ -26737,7 +27216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051BD652-3ACC-C74A-8467-89B1A58FDD59}">
   <dimension ref="A1:N24"/>
   <sheetViews>
@@ -27486,12 +27965,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247C162A-248F-4A45-BE61-8540424C7CFA}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27600,12 +28079,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="A1:XFD1048576"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27732,7 +28211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -27864,7 +28343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -27997,7 +28476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -28130,140 +28609,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2.5299999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2.5299999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3.22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>6.77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>3.44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>6.35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2.81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3.71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <f>SUM(B3:B14)</f>
-        <v>51.59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>